<commit_message>
feat:reset system: selections, reports and students
</commit_message>
<xml_diff>
--- a/static/file/supTopic_example.xlsx
+++ b/static/file/supTopic_example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9060"/>
+    <workbookView windowWidth="18348" windowHeight="6900"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Staff member</t>
   </si>
@@ -38,10 +38,10 @@
     <t>Proposed Titles</t>
   </si>
   <si>
-    <t>Topic details</t>
-  </si>
-  <si>
-    <t>Required skills</t>
+    <t xml:space="preserve">Topic details </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Required skills </t>
   </si>
   <si>
     <t>References</t>
@@ -64,7 +64,26 @@
 2.        Implement the most efficient model.</t>
   </si>
   <si>
-    <t>Programming skills in at least Python, preferably experience with deep learning coding frameworks like PyTorch, or Tensorflow;  Some knowledge of machine learning applied to recommender systems.</t>
+    <r>
+      <t xml:space="preserve">Programming skills in at least Python, preferably experience with deep learning coding frameworks like PyTorch, or Tensorflow;  Some knowledge of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>machine learning</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> applied to recommender systems.</t>
+    </r>
   </si>
   <si>
     <t>Project resources to be given later</t>
@@ -78,34 +97,39 @@
 2.        Implement the most efficient model.</t>
   </si>
   <si>
-    <t>Clivia Li</t>
-  </si>
-  <si>
-    <t>Advanced Web Applications, Information Systems, Software Development, Wechat Mini-programs</t>
-  </si>
-  <si>
-    <t>Collaborative Code Editor</t>
-  </si>
-  <si>
-    <t>This project aims to create a web application that enables multiple users to collaboratively write and edit code in real-time. It provides an interactive and seamless environment where developers can work together on coding projects, troubleshoot issues, and share their knowledge efficiently. Key features include a code editor interface where users can write, edit, and save code with changes made by multiple users synchronized in real-time, a chat or messaging system to facilitate communication, and code execution and testing capabilities to run code snippets and display output and errors.</t>
-  </si>
-  <si>
-    <t>Web frontend and backend skills; user authentication; real-time communication; database skills</t>
-  </si>
-  <si>
-    <t>https://geekflare.com/best-collaborative-coding-tools/</t>
-  </si>
-  <si>
-    <t>Task Management Tool for Agile Projects</t>
-  </si>
-  <si>
-    <t>This project aims to develop a web application that helps software development teams engaged in an agile project to manage their tasks and workflow. It allows the user to put together a product backlog, build their sprint plans, break down user stories to tasks, and assign tasks to team members. It provides autocorrection and suggestion for the phrasing and content of user stories.</t>
-  </si>
-  <si>
-    <t>Web frontend and backend skills; user authentication; database skills</t>
-  </si>
-  <si>
-    <t>https://www.proofhub.com/articles/agile-project-management-tools-list</t>
+    <t>Programming skills in at least Python, preferably experience with deep learning coding frameworks like PyTorch, or Tensorflow;  Some knowledge of machine learning applied to recommender systems.</t>
+  </si>
+  <si>
+    <t>Albert Xu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deep Learning, Information Systems,web-based systems </t>
+  </si>
+  <si>
+    <t>Deep Learning-Based Medical Image Diagnosis System</t>
+  </si>
+  <si>
+    <t>Develop a deep learning system that can automatically analyze medical images (such as X-rays, MRI, CT scans) to detect diseases like pneumonia, tumors, etc.</t>
+  </si>
+  <si>
+    <t>Deep Learning Frameworks (TensorFlow, PyTorch)
+Medical Image Processing (CNN, U-Net)
+Data Annotation and Preprocessing</t>
+  </si>
+  <si>
+    <t>Rajpurkar P, et al. CheXNet: Radiologist-level pneumonia detection on chest X-rays with deep learning.</t>
+  </si>
+  <si>
+    <t>Multi-Objective Segmentation of Joystick Maps Based on Deep Learning</t>
+  </si>
+  <si>
+    <t>Multi-Objective Identification of Features in High-Resolution Remote Sensing Satellite Maps using Deep Learning: Road, Building, Water Body, Farmland, and More.</t>
+  </si>
+  <si>
+    <t>Python Programming,Deep Learning Frameworks: Familiarity with deep learning frameworks like TensorFlow, PyTorch.etc</t>
+  </si>
+  <si>
+    <t>Sun Y, Hu J, Yun J, et al. Multi-objective location and mapping based on deep learning and visual slam[J]. Sensors, 2022, 22(19): 7576.</t>
   </si>
 </sst>
 </file>
@@ -118,7 +142,7 @@
     <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,12 +170,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
       <sz val="12"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -647,137 +665,137 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -802,23 +820,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1141,7 +1162,7 @@
   <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4"/>
@@ -1178,23 +1199,23 @@
       <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
     </row>
     <row r="2" s="2" customFormat="1" ht="60" spans="1:7">
       <c r="A2" s="7" t="s">
@@ -1233,7 +1254,7 @@
         <v>14</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>12</v>
@@ -1242,56 +1263,53 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="135" spans="1:7">
+    <row r="4" s="2" customFormat="1" ht="45" spans="1:7">
       <c r="A4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="B4" s="13" t="s">
         <v>17</v>
       </c>
+      <c r="C4" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="D4" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="11">
-        <v>2</v>
+      <c r="F4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="14">
+        <v>1</v>
       </c>
     </row>
-    <row r="5" ht="90" spans="1:7">
+    <row r="5" s="2" customFormat="1" ht="45" spans="1:7">
       <c r="A5" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>21</v>
+      <c r="B5" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="11">
-        <v>2</v>
+      <c r="F5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="14">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" display="https://geekflare.com/best-collaborative-coding-tools/"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>